<commit_message>
revisi abis acc bu rahmi - perbaiki abstrak, tambah b.ing, tambah lembar pengesahan, perbaiki rumusan masalah, hapus wm fritzing
</commit_message>
<xml_diff>
--- a/Pengujian sistem.xlsx
+++ b/Pengujian sistem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Skripsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E338F83-EB27-46C7-8F2E-967937590A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFCD866-1D5B-43F1-9EDF-7F311E83555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{428DB996-DF06-4436-9777-2812E9C7A93C}"/>
   </bookViews>
@@ -274,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -325,9 +325,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -340,34 +370,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -690,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E9BF61-3413-4B01-8309-C75059EF9CE1}">
   <dimension ref="A1:AL40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3:R13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -710,7 +713,7 @@
     <col min="12" max="12" width="7.5546875" customWidth="1"/>
     <col min="13" max="13" width="10.109375" customWidth="1"/>
     <col min="14" max="14" width="10.6640625" customWidth="1"/>
-    <col min="15" max="15" width="6.21875" customWidth="1"/>
+    <col min="15" max="15" width="8" customWidth="1"/>
     <col min="16" max="16" width="7.88671875" customWidth="1"/>
     <col min="17" max="17" width="8.6640625" customWidth="1"/>
     <col min="18" max="18" width="8.109375" customWidth="1"/>
@@ -880,7 +883,7 @@
         <v>39</v>
       </c>
       <c r="O3" s="1">
-        <f>ABS(M3-N3)</f>
+        <f>(N3-M3)</f>
         <v>0.60000000000000142</v>
       </c>
       <c r="P3" s="2">
@@ -894,7 +897,7 @@
       <c r="V3" s="4">
         <v>1</v>
       </c>
-      <c r="W3" s="19" t="s">
+      <c r="W3" s="29" t="s">
         <v>29</v>
       </c>
       <c r="X3" s="4">
@@ -976,11 +979,11 @@
         <v>39.6</v>
       </c>
       <c r="O4" s="1">
-        <f t="shared" ref="O4:O13" si="0">ABS(M4-N4)</f>
+        <f t="shared" ref="O4:O13" si="0">(N4-M4)</f>
         <v>0.70000000000000284</v>
       </c>
       <c r="P4" s="2">
-        <f t="shared" ref="P4:P13" si="1">ABS(((M4-N4)/N4)*100%)</f>
+        <f t="shared" ref="P4:P12" si="1">ABS(((M4-N4)/N4)*100%)</f>
         <v>1.7676767676767749E-2</v>
       </c>
       <c r="Q4" s="2">
@@ -990,7 +993,7 @@
       <c r="V4" s="4">
         <v>2</v>
       </c>
-      <c r="W4" s="19"/>
+      <c r="W4" s="29"/>
       <c r="X4" s="4">
         <v>20</v>
       </c>
@@ -1084,7 +1087,7 @@
       <c r="V5" s="4">
         <v>3</v>
       </c>
-      <c r="W5" s="19"/>
+      <c r="W5" s="29"/>
       <c r="X5" s="4">
         <v>30</v>
       </c>
@@ -1158,22 +1161,22 @@
         <v>20</v>
       </c>
       <c r="M6" s="1">
-        <v>40.5</v>
+        <v>40.1</v>
       </c>
       <c r="N6" s="1">
         <v>40.1</v>
       </c>
       <c r="O6" s="1">
         <f t="shared" si="0"/>
-        <v>0.39999999999999858</v>
+        <v>0</v>
       </c>
       <c r="P6" s="2">
         <f t="shared" si="1"/>
-        <v>9.9750623441396159E-3</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="2">
         <f t="shared" si="2"/>
-        <v>0.99002493765586042</v>
+        <v>1</v>
       </c>
       <c r="R6">
         <v>2.17</v>
@@ -1181,7 +1184,7 @@
       <c r="V6" s="4">
         <v>4</v>
       </c>
-      <c r="W6" s="19"/>
+      <c r="W6" s="29"/>
       <c r="X6" s="4">
         <v>40</v>
       </c>
@@ -1278,7 +1281,7 @@
       <c r="V7" s="4">
         <v>5</v>
       </c>
-      <c r="W7" s="19"/>
+      <c r="W7" s="29"/>
       <c r="X7" s="4">
         <v>50</v>
       </c>
@@ -1375,7 +1378,7 @@
       <c r="V8" s="4">
         <v>6</v>
       </c>
-      <c r="W8" s="19" t="s">
+      <c r="W8" s="29" t="s">
         <v>30</v>
       </c>
       <c r="X8" s="4">
@@ -1474,7 +1477,7 @@
       <c r="V9" s="4">
         <v>7</v>
       </c>
-      <c r="W9" s="19"/>
+      <c r="W9" s="29"/>
       <c r="X9" s="4">
         <v>20</v>
       </c>
@@ -1571,7 +1574,7 @@
       <c r="V10" s="4">
         <v>8</v>
       </c>
-      <c r="W10" s="19"/>
+      <c r="W10" s="29"/>
       <c r="X10" s="4">
         <v>30</v>
       </c>
@@ -1668,7 +1671,7 @@
       <c r="V11" s="4">
         <v>9</v>
       </c>
-      <c r="W11" s="19"/>
+      <c r="W11" s="29"/>
       <c r="X11" s="4">
         <v>40</v>
       </c>
@@ -1748,7 +1751,7 @@
         <v>46.3</v>
       </c>
       <c r="O12" s="1">
-        <f>ABS(M12-N12)</f>
+        <f t="shared" si="0"/>
         <v>0.69999999999999574</v>
       </c>
       <c r="P12" s="2">
@@ -1765,7 +1768,7 @@
       <c r="V12" s="4">
         <v>10</v>
       </c>
-      <c r="W12" s="19"/>
+      <c r="W12" s="29"/>
       <c r="X12" s="4">
         <v>50</v>
       </c>
@@ -1811,14 +1814,14 @@
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
       <c r="G13" s="1">
         <f>AVERAGE(G3:G12)</f>
         <v>4.0350000000000001</v>
@@ -1829,17 +1832,17 @@
       <c r="L13" s="25"/>
       <c r="M13" s="25"/>
       <c r="N13" s="26"/>
-      <c r="O13" s="1">
+      <c r="O13" s="33">
         <f>AVERAGE(O3:O12)</f>
-        <v>0.67000000000000026</v>
+        <v>0.63000000000000045</v>
       </c>
       <c r="P13" s="2">
         <f>AVERAGE(P3:P12)</f>
-        <v>1.575473750160598E-2</v>
+        <v>1.4757231267192023E-2</v>
       </c>
       <c r="Q13" s="2">
         <f>AVERAGE(Q3:Q12)</f>
-        <v>0.98424526249839395</v>
+        <v>0.98524276873280792</v>
       </c>
       <c r="R13" s="16">
         <f>AVERAGE(R3:R12)</f>
@@ -1848,7 +1851,7 @@
       <c r="V13" s="4">
         <v>11</v>
       </c>
-      <c r="W13" s="19" t="s">
+      <c r="W13" s="29" t="s">
         <v>31</v>
       </c>
       <c r="X13" s="4">
@@ -1900,7 +1903,7 @@
       <c r="V14" s="4">
         <v>12</v>
       </c>
-      <c r="W14" s="19"/>
+      <c r="W14" s="29"/>
       <c r="X14" s="4">
         <v>20</v>
       </c>
@@ -1955,7 +1958,7 @@
       <c r="V15" s="4">
         <v>13</v>
       </c>
-      <c r="W15" s="19"/>
+      <c r="W15" s="29"/>
       <c r="X15" s="4">
         <v>30</v>
       </c>
@@ -2006,14 +2009,14 @@
       <c r="B16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23" t="s">
+      <c r="D16" s="28"/>
+      <c r="E16" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="23"/>
+      <c r="F16" s="28"/>
       <c r="K16" s="3" t="s">
         <v>1</v>
       </c>
@@ -2036,7 +2039,7 @@
       <c r="V16" s="4">
         <v>14</v>
       </c>
-      <c r="W16" s="19"/>
+      <c r="W16" s="29"/>
       <c r="X16" s="11">
         <v>40</v>
       </c>
@@ -2087,37 +2090,37 @@
       <c r="B17" s="1">
         <v>10</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="18"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="27"/>
       <c r="K17" s="1">
         <v>1</v>
       </c>
-      <c r="L17" s="27">
+      <c r="L17" s="21">
         <v>30</v>
       </c>
-      <c r="M17" s="28"/>
+      <c r="M17" s="23"/>
       <c r="N17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O17" s="27" t="s">
+      <c r="O17" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="27" t="s">
+      <c r="P17" s="23"/>
+      <c r="Q17" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="R17" s="29"/>
-      <c r="S17" s="28"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="23"/>
       <c r="V17" s="4">
         <v>15</v>
       </c>
-      <c r="W17" s="19"/>
+      <c r="W17" s="29"/>
       <c r="X17" s="11">
         <v>50</v>
       </c>
@@ -2168,55 +2171,55 @@
       <c r="B18" s="1">
         <v>10</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18" t="s">
+      <c r="D18" s="27"/>
+      <c r="E18" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="18"/>
+      <c r="F18" s="27"/>
       <c r="K18" s="1">
         <v>2</v>
       </c>
-      <c r="L18" s="27">
+      <c r="L18" s="21">
         <v>35</v>
       </c>
-      <c r="M18" s="28"/>
+      <c r="M18" s="23"/>
       <c r="N18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O18" s="27" t="s">
+      <c r="O18" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="27" t="s">
+      <c r="P18" s="23"/>
+      <c r="Q18" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="R18" s="29"/>
-      <c r="S18" s="28"/>
-      <c r="V18" s="20" t="s">
+      <c r="R18" s="22"/>
+      <c r="S18" s="23"/>
+      <c r="V18" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="W18" s="21"/>
-      <c r="X18" s="21"/>
-      <c r="Y18" s="21"/>
-      <c r="Z18" s="21"/>
-      <c r="AA18" s="22"/>
+      <c r="W18" s="31"/>
+      <c r="X18" s="31"/>
+      <c r="Y18" s="31"/>
+      <c r="Z18" s="31"/>
+      <c r="AA18" s="32"/>
       <c r="AB18" s="12">
         <f>AVERAGE(AB3:AB17)</f>
         <v>2.9893333333333336</v>
       </c>
-      <c r="AD18" s="18" t="s">
+      <c r="AD18" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="AE18" s="18"/>
-      <c r="AF18" s="18"/>
-      <c r="AG18" s="18"/>
-      <c r="AH18" s="18"/>
-      <c r="AI18" s="18"/>
-      <c r="AJ18" s="18"/>
-      <c r="AK18" s="18"/>
+      <c r="AE18" s="27"/>
+      <c r="AF18" s="27"/>
+      <c r="AG18" s="27"/>
+      <c r="AH18" s="27"/>
+      <c r="AI18" s="27"/>
+      <c r="AJ18" s="27"/>
+      <c r="AK18" s="27"/>
       <c r="AL18" s="12">
         <f>AVERAGE(AL3:AL17)</f>
         <v>2.3692307692307693</v>
@@ -2226,22 +2229,22 @@
       <c r="K19" s="1">
         <v>3</v>
       </c>
-      <c r="L19" s="27">
+      <c r="L19" s="21">
         <v>40</v>
       </c>
-      <c r="M19" s="28"/>
+      <c r="M19" s="23"/>
       <c r="N19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O19" s="27" t="s">
+      <c r="O19" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="27">
+      <c r="P19" s="23"/>
+      <c r="Q19" s="21">
         <v>2.17</v>
       </c>
-      <c r="R19" s="29"/>
-      <c r="S19" s="28"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="23"/>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B20">
@@ -2253,22 +2256,22 @@
       <c r="K20" s="1">
         <v>4</v>
       </c>
-      <c r="L20" s="27">
+      <c r="L20" s="21">
         <v>45</v>
       </c>
-      <c r="M20" s="28"/>
+      <c r="M20" s="23"/>
       <c r="N20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O20" s="27" t="s">
+      <c r="O20" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="27">
+      <c r="P20" s="23"/>
+      <c r="Q20" s="21">
         <v>2.72</v>
       </c>
-      <c r="R20" s="29"/>
-      <c r="S20" s="28"/>
+      <c r="R20" s="22"/>
+      <c r="S20" s="23"/>
       <c r="X20" s="4">
         <v>10</v>
       </c>
@@ -2289,22 +2292,22 @@
       <c r="K21" s="1">
         <v>5</v>
       </c>
-      <c r="L21" s="27">
+      <c r="L21" s="21">
         <v>50</v>
       </c>
-      <c r="M21" s="28"/>
+      <c r="M21" s="23"/>
       <c r="N21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O21" s="27" t="s">
+      <c r="O21" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="P21" s="28"/>
-      <c r="Q21" s="27">
+      <c r="P21" s="23"/>
+      <c r="Q21" s="21">
         <v>2.42</v>
       </c>
-      <c r="R21" s="29"/>
-      <c r="S21" s="28"/>
+      <c r="R21" s="22"/>
+      <c r="S21" s="23"/>
       <c r="X21" s="4">
         <v>20</v>
       </c>
@@ -2325,22 +2328,22 @@
       <c r="K22" s="1">
         <v>6</v>
       </c>
-      <c r="L22" s="27">
+      <c r="L22" s="21">
         <v>55</v>
       </c>
-      <c r="M22" s="28"/>
+      <c r="M22" s="23"/>
       <c r="N22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O22" s="27" t="s">
+      <c r="O22" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="27">
+      <c r="P22" s="23"/>
+      <c r="Q22" s="21">
         <v>2.83</v>
       </c>
-      <c r="R22" s="29"/>
-      <c r="S22" s="28"/>
+      <c r="R22" s="22"/>
+      <c r="S22" s="23"/>
       <c r="X22" s="4">
         <v>30</v>
       </c>
@@ -2361,22 +2364,22 @@
       <c r="K23" s="1">
         <v>7</v>
       </c>
-      <c r="L23" s="27">
+      <c r="L23" s="21">
         <v>60</v>
       </c>
-      <c r="M23" s="28"/>
+      <c r="M23" s="23"/>
       <c r="N23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O23" s="27" t="s">
+      <c r="O23" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="P23" s="28"/>
-      <c r="Q23" s="27">
+      <c r="P23" s="23"/>
+      <c r="Q23" s="21">
         <v>2.57</v>
       </c>
-      <c r="R23" s="29"/>
-      <c r="S23" s="28"/>
+      <c r="R23" s="22"/>
+      <c r="S23" s="23"/>
       <c r="X23" s="4">
         <v>40</v>
       </c>
@@ -2391,22 +2394,22 @@
       <c r="K24" s="1">
         <v>8</v>
       </c>
-      <c r="L24" s="27">
+      <c r="L24" s="21">
         <v>65</v>
       </c>
-      <c r="M24" s="28"/>
+      <c r="M24" s="23"/>
       <c r="N24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O24" s="27" t="s">
+      <c r="O24" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="P24" s="28"/>
-      <c r="Q24" s="27">
+      <c r="P24" s="23"/>
+      <c r="Q24" s="21">
         <v>2.5</v>
       </c>
-      <c r="R24" s="29"/>
-      <c r="S24" s="28"/>
+      <c r="R24" s="22"/>
+      <c r="S24" s="23"/>
       <c r="X24" s="4">
         <v>50</v>
       </c>
@@ -2421,22 +2424,22 @@
       <c r="K25" s="1">
         <v>9</v>
       </c>
-      <c r="L25" s="27">
+      <c r="L25" s="21">
         <v>70</v>
       </c>
-      <c r="M25" s="28"/>
+      <c r="M25" s="23"/>
       <c r="N25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O25" s="27" t="s">
+      <c r="O25" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="P25" s="28"/>
-      <c r="Q25" s="27">
+      <c r="P25" s="23"/>
+      <c r="Q25" s="21">
         <v>3.32</v>
       </c>
-      <c r="R25" s="29"/>
-      <c r="S25" s="28"/>
+      <c r="R25" s="22"/>
+      <c r="S25" s="23"/>
       <c r="X25" s="4">
         <v>60</v>
       </c>
@@ -2451,22 +2454,22 @@
       <c r="K26" s="1">
         <v>10</v>
       </c>
-      <c r="L26" s="27">
+      <c r="L26" s="21">
         <v>75</v>
       </c>
-      <c r="M26" s="28"/>
+      <c r="M26" s="23"/>
       <c r="N26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O26" s="27" t="s">
+      <c r="O26" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="P26" s="28"/>
-      <c r="Q26" s="27">
+      <c r="P26" s="23"/>
+      <c r="Q26" s="21">
         <v>3</v>
       </c>
-      <c r="R26" s="29"/>
-      <c r="S26" s="28"/>
+      <c r="R26" s="22"/>
+      <c r="S26" s="23"/>
       <c r="X26" s="4">
         <v>70</v>
       </c>
@@ -2486,12 +2489,12 @@
       <c r="N27" s="25"/>
       <c r="O27" s="25"/>
       <c r="P27" s="26"/>
-      <c r="Q27" s="30">
+      <c r="Q27" s="18">
         <f>AVERAGE(Q17:S26)</f>
         <v>2.6912500000000001</v>
       </c>
-      <c r="R27" s="31"/>
-      <c r="S27" s="32"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="20"/>
       <c r="X27" s="4">
         <v>80</v>
       </c>
@@ -2642,12 +2645,32 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="Q27:S27"/>
-    <mergeCell ref="Q22:S22"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="Q24:S24"/>
-    <mergeCell ref="Q25:S25"/>
-    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="AD18:AK18"/>
+    <mergeCell ref="W3:W7"/>
+    <mergeCell ref="W8:W12"/>
+    <mergeCell ref="W13:W17"/>
+    <mergeCell ref="V18:AA18"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="L18:M18"/>
     <mergeCell ref="K27:P27"/>
     <mergeCell ref="O16:P16"/>
     <mergeCell ref="O17:P17"/>
@@ -2664,32 +2687,12 @@
     <mergeCell ref="L23:M23"/>
     <mergeCell ref="L24:M24"/>
     <mergeCell ref="L25:M25"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="AD18:AK18"/>
-    <mergeCell ref="W3:W7"/>
-    <mergeCell ref="W8:W12"/>
-    <mergeCell ref="W13:W17"/>
-    <mergeCell ref="V18:AA18"/>
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="Q22:S22"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="Q25:S25"/>
+    <mergeCell ref="Q26:S26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
revisi skripsi abis semhas + jurnal
</commit_message>
<xml_diff>
--- a/Pengujian sistem.xlsx
+++ b/Pengujian sistem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Skripsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFCD866-1D5B-43F1-9EDF-7F311E83555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30D3C26-8BB3-4E44-816C-6BCFB5806644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{428DB996-DF06-4436-9777-2812E9C7A93C}"/>
   </bookViews>
@@ -274,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -369,9 +369,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -691,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E9BF61-3413-4B01-8309-C75059EF9CE1}">
-  <dimension ref="A1:AL40"/>
+  <dimension ref="A1:AL52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" topLeftCell="S22" zoomScale="102" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Y48" sqref="Y48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -979,7 +976,7 @@
         <v>39.6</v>
       </c>
       <c r="O4" s="1">
-        <f t="shared" ref="O4:O13" si="0">(N4-M4)</f>
+        <f t="shared" ref="O4:O12" si="0">(N4-M4)</f>
         <v>0.70000000000000284</v>
       </c>
       <c r="P4" s="2">
@@ -1832,7 +1829,7 @@
       <c r="L13" s="25"/>
       <c r="M13" s="25"/>
       <c r="N13" s="26"/>
-      <c r="O13" s="33">
+      <c r="O13" s="1">
         <f>AVERAGE(O3:O12)</f>
         <v>0.63000000000000045</v>
       </c>
@@ -2641,6 +2638,98 @@
       <c r="AB40" s="16">
         <f>AVERAGE(AB20:AB37)</f>
         <v>2.835294117647059</v>
+      </c>
+    </row>
+    <row r="43" spans="24:28" x14ac:dyDescent="0.3">
+      <c r="X43" s="4">
+        <v>10</v>
+      </c>
+      <c r="Y43">
+        <v>1446.55</v>
+      </c>
+      <c r="Z43">
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="44" spans="24:28" x14ac:dyDescent="0.3">
+      <c r="X44" s="4">
+        <v>20</v>
+      </c>
+      <c r="Y44">
+        <v>835.66</v>
+      </c>
+      <c r="Z44">
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="45" spans="24:28" x14ac:dyDescent="0.3">
+      <c r="X45" s="4">
+        <v>30</v>
+      </c>
+      <c r="Y45">
+        <v>704.13</v>
+      </c>
+      <c r="Z45">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="46" spans="24:28" x14ac:dyDescent="0.3">
+      <c r="X46" s="4">
+        <v>40</v>
+      </c>
+      <c r="Y46">
+        <v>405.08</v>
+      </c>
+      <c r="Z46">
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="47" spans="24:28" x14ac:dyDescent="0.3">
+      <c r="X47" s="4">
+        <v>50</v>
+      </c>
+      <c r="Y47">
+        <v>316.49</v>
+      </c>
+      <c r="Z47">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="48" spans="24:28" x14ac:dyDescent="0.3">
+      <c r="X48" s="4">
+        <v>60</v>
+      </c>
+      <c r="Y48">
+        <v>343.96</v>
+      </c>
+      <c r="Z48">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="49" spans="24:26" x14ac:dyDescent="0.3">
+      <c r="X49" s="4">
+        <v>70</v>
+      </c>
+      <c r="Y49">
+        <v>1319.71</v>
+      </c>
+      <c r="Z49">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="50" spans="24:26" x14ac:dyDescent="0.3">
+      <c r="X50" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="24:26" x14ac:dyDescent="0.3">
+      <c r="X51" s="4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="24:26" x14ac:dyDescent="0.3">
+      <c r="X52" s="4">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>